<commit_message>
Execute Tests on Android mobile browser
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/BecomePartnerPage.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/BecomePartnerPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhinav\IdeaProjects\CouchBase\src\main\resources\CompilerDictionary\LocatorDictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/Mobile-Web-Automation/src/main/resources/CompilerDictionary/LocatorDictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F580445A-6E24-476D-AA7B-8D77BFC76877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EAFF1E-2FDE-D84D-B73D-908CC81E95B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BecomePartnerPage" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>Sno</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>//a[contains(text(),'Couchbase Master Partner Agreement')]/parent::span/ancestor::div/input</t>
+  </si>
+  <si>
+    <t>Locator Type</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Xpath</t>
   </si>
 </sst>
 </file>
@@ -609,20 +618,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,8 +642,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -643,8 +656,11 @@
       <c r="C2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -654,8 +670,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -665,8 +684,11 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -676,8 +698,11 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -687,8 +712,11 @@
       <c r="C6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -698,8 +726,11 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -709,8 +740,11 @@
       <c r="C8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -720,8 +754,11 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -731,8 +768,11 @@
       <c r="C10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -742,8 +782,11 @@
       <c r="C11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -753,8 +796,11 @@
       <c r="C12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -764,8 +810,11 @@
       <c r="C13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -775,8 +824,11 @@
       <c r="C14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -786,8 +838,11 @@
       <c r="C15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -797,8 +852,11 @@
       <c r="C16" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -808,8 +866,11 @@
       <c r="C17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -819,8 +880,11 @@
       <c r="C18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -830,8 +894,11 @@
       <c r="C19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -841,8 +908,11 @@
       <c r="C20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -852,8 +922,11 @@
       <c r="C21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -863,8 +936,11 @@
       <c r="C22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -874,8 +950,11 @@
       <c r="C23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -885,8 +964,11 @@
       <c r="C24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -896,8 +978,11 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -907,8 +992,11 @@
       <c r="C26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -918,8 +1006,11 @@
       <c r="C27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -929,8 +1020,11 @@
       <c r="C28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -940,8 +1034,11 @@
       <c r="C29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -951,8 +1048,11 @@
       <c r="C30" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -962,8 +1062,11 @@
       <c r="C31" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -973,8 +1076,11 @@
       <c r="C32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -984,8 +1090,11 @@
       <c r="C33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -995,8 +1104,11 @@
       <c r="C34" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1006,8 +1118,11 @@
       <c r="C35" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1017,8 +1132,11 @@
       <c r="C36" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1028,8 +1146,11 @@
       <c r="C37" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1039,8 +1160,11 @@
       <c r="C38" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1049,6 +1173,9 @@
       </c>
       <c r="C39" t="s">
         <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1192,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1077,7 +1204,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>